<commit_message>
Updating script to create thread, formatted tweets, added quality control checks.
</commit_message>
<xml_diff>
--- a/data/candidate_list.xlsx
+++ b/data/candidate_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wichman/Dropbox/tweetwomen/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wichman/Documents/tweetwomenjmc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224D6A3F-6DBF-C445-B3D6-DF67C6DB1122}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7000686B-ADB1-0448-A987-A9697D9BA102}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5860" yWindow="2200" windowWidth="19080" windowHeight="11200" xr2:uid="{3C8774B2-D5DE-6845-86D5-1B0B4BAD2E30}"/>
+    <workbookView xWindow="80" yWindow="4000" windowWidth="19080" windowHeight="11200" xr2:uid="{3C8774B2-D5DE-6845-86D5-1B0B4BAD2E30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -67,6 +67,30 @@
   </si>
   <si>
     <t>Bankruptcy Policy</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>Econ</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>This is a really long JMP title to test character limits: Evidence from a randomized control trial</t>
+  </si>
+  <si>
+    <t>https://www.twitter.com/</t>
+  </si>
+  <si>
+    <t>University of Phoenix</t>
+  </si>
+  <si>
+    <t>posted</t>
+  </si>
+  <si>
+    <t>qflag</t>
   </si>
 </sst>
 </file>
@@ -429,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58BB7AAB-33B5-1547-A4EE-562917F35D9E}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,9 +464,10 @@
     <col min="1" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,8 +480,17 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -469,8 +503,17 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -482,12 +525,45 @@
       </c>
       <c r="D3" t="s">
         <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{8C6703D7-6357-AD4D-9F6A-BC14052C7012}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{ECB3B161-2C48-0E4D-8D8B-3D44834C6BC6}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{DE5CDE49-615D-8B4C-9EEA-9AB589B0FD5E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>